<commit_message>
feat(files): add Result_Sheet.xlsx and remove Marksheet_test.xlsx
- Added new binary file Result_Sheet.xlsx to the project
- Removed obsolete binary file Marksheet_test.xlsx from the project
</commit_message>
<xml_diff>
--- a/Result_Sheet.xlsx
+++ b/Result_Sheet.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,9 @@
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="31" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="9" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -519,30 +516,15 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Q1 (6)</t>
+          <t>Total Marks</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>Q2 (6)</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>Q3 (8)</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>Total Marks</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-      <c r="J8" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -565,26 +547,17 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>11.5</v>
       </c>
       <c r="E9" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8</v>
-      </c>
-      <c r="G9" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="H9" t="n">
         <v>20</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>57.5%</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
@@ -607,26 +580,17 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>14</v>
-      </c>
-      <c r="H10" t="n">
         <v>20</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>70.0%</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
@@ -649,26 +613,17 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>8</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14</v>
-      </c>
-      <c r="H11" t="n">
         <v>20</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>70.0%</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
@@ -691,26 +646,17 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" t="n">
-        <v>13</v>
-      </c>
-      <c r="H12" t="n">
         <v>20</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>65.0%</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
@@ -733,26 +679,17 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" t="n">
-        <v>14</v>
-      </c>
-      <c r="H13" t="n">
         <v>20</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>70.0%</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Checked</t>
         </is>
@@ -774,22 +711,20 @@
           <t>prn-2222521242026@college.edu</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Not Graded</t>
-        </is>
+      <c r="D14" t="n">
+        <v>6</v>
       </c>
       <c r="E14" t="n">
         <v>20</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>30.0%</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Checked</t>
         </is>
       </c>
     </row>

</xml_diff>